<commit_message>
Fehler bei berechneten Feldern
</commit_message>
<xml_diff>
--- a/dolibarr-skr49 EUeR.xlsx
+++ b/dolibarr-skr49 EUeR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannes/Documents/Programming/Innwerk/dolibarr-kontenplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88D5699-E220-324C-8BA9-7C9D31BA6517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BBE6EC-104B-8F43-BD57-24E4D4EBA80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30820" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKR49" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3520" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3519" uniqueCount="883">
   <si>
     <t>Kontenplan</t>
   </si>
@@ -2290,36 +2290,6 @@
     <t>INCOME</t>
   </si>
   <si>
-    <t>IBEIN-1</t>
-  </si>
-  <si>
-    <t>IBEIN-2</t>
-  </si>
-  <si>
-    <t>IBEIN-3</t>
-  </si>
-  <si>
-    <t>IBEIN-4</t>
-  </si>
-  <si>
-    <t>IBAUS-1</t>
-  </si>
-  <si>
-    <t>IBAUS-2</t>
-  </si>
-  <si>
-    <t>IBAUS-3</t>
-  </si>
-  <si>
-    <t>IBAUS-4</t>
-  </si>
-  <si>
-    <t>IBAUS-5</t>
-  </si>
-  <si>
-    <t>IBAUS-6</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -2368,33 +2338,18 @@
     <t>Zuschüsse</t>
   </si>
   <si>
-    <t>IBEIN-5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige steuerneutrale Einnahmen </t>
   </si>
   <si>
-    <t>IBEIN-6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Schenkungen </t>
   </si>
   <si>
-    <t>IBEIN-7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Erbschaften/ Vermächtnisse </t>
   </si>
   <si>
-    <t>IBEIN-8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spenden </t>
   </si>
   <si>
-    <t>IBEIN-9</t>
-  </si>
-  <si>
     <t xml:space="preserve">Steuerneutrale Einnahmen </t>
   </si>
   <si>
@@ -2419,24 +2374,12 @@
     <t xml:space="preserve">Raumkosten </t>
   </si>
   <si>
-    <t>IBAUS-7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige nicht abziehbare Ausgaben </t>
   </si>
   <si>
-    <t>IBAUS-8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gezahlte/hingegebene Spenden </t>
   </si>
   <si>
-    <t>IBAUS-9</t>
-  </si>
-  <si>
-    <t>IBAUS-10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nicht abziehbare Ausgaben </t>
   </si>
   <si>
@@ -2446,72 +2389,33 @@
     <t>Zweckbetrieb</t>
   </si>
   <si>
-    <t>ZBEIN-1</t>
-  </si>
-  <si>
-    <t>ZBEIN-2</t>
-  </si>
-  <si>
-    <t>ZBEIN-3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Andere aktivierte Eigenleistungen </t>
   </si>
   <si>
-    <t>ZBEIN-4</t>
-  </si>
-  <si>
     <t>ZBAUS</t>
   </si>
   <si>
-    <t>ZBAUS-1</t>
-  </si>
-  <si>
-    <t>ZBAUS-2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aufwendungen für bezogene Leistungen </t>
   </si>
   <si>
-    <t>ZBAUS-3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Löhne und Gehälter </t>
   </si>
   <si>
-    <t>ZBAUS-4</t>
-  </si>
-  <si>
     <t>Soziale Abgaben</t>
   </si>
   <si>
-    <t>ZBAUS-5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Immaterielle Vermögensgegenstände und Sachanlagen </t>
   </si>
   <si>
-    <t>ZBAUS-6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Umlaufvermögen, unüblich hoch </t>
   </si>
   <si>
-    <t>ZBAUS-7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige betriebliche Aufwendungen </t>
   </si>
   <si>
-    <t>ZBAUS-8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Zinsen und ähnliche Aufwendungen </t>
   </si>
   <si>
-    <t>ZBAUS-9</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige Steuern </t>
   </si>
   <si>
@@ -2521,93 +2425,39 @@
     <t>Geschäftsbetrieb</t>
   </si>
   <si>
-    <t>GBEIN-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Umsatzerlöse </t>
   </si>
   <si>
-    <t>GBEIN-2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige betriebliche Erträge </t>
   </si>
   <si>
-    <t>GBEIN-3</t>
-  </si>
-  <si>
-    <t>GBEIN-4</t>
-  </si>
-  <si>
-    <t>GBEIN-5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige Zinsen und ähnliche Einnahmen </t>
   </si>
   <si>
     <t>GBAUS</t>
   </si>
   <si>
-    <t>GBAUS-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ausgaben für Roh-, Hilfs- und Betriebsstoffe und für bezogene Waren </t>
   </si>
   <si>
-    <t>GBAUS-2</t>
-  </si>
-  <si>
-    <t>GBAUS-3</t>
-  </si>
-  <si>
-    <t>GBAUS-4</t>
-  </si>
-  <si>
-    <t>GBAUS-5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Soziale Abgaben </t>
   </si>
   <si>
-    <t>GBAUS-6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Immaterielle Vermögensgegenstände und Sachanlagen </t>
   </si>
   <si>
-    <t>GBAUS-7</t>
-  </si>
-  <si>
-    <t>GBAUS-8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Erträge aus Beteiligungen </t>
   </si>
   <si>
-    <t>GBAUS-9</t>
-  </si>
-  <si>
     <t xml:space="preserve">Erträge aus anderen Wertpapieren </t>
   </si>
   <si>
-    <t>GBAUS-10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige Zinsen und ähnliche Erträge </t>
   </si>
   <si>
-    <t>GBAUS-11</t>
-  </si>
-  <si>
     <t xml:space="preserve">Abschreibungen auf Finanzanlagen </t>
   </si>
   <si>
-    <t>GBAUS-12</t>
-  </si>
-  <si>
-    <t>GBAUS-13</t>
-  </si>
-  <si>
     <t>Übrige Ausgaben</t>
   </si>
   <si>
@@ -2671,43 +2521,190 @@
     <t>VVEIN</t>
   </si>
   <si>
-    <t>VVEIN-1</t>
-  </si>
-  <si>
-    <t>VVEIN-2</t>
-  </si>
-  <si>
-    <t>VVEIN-3</t>
-  </si>
-  <si>
-    <t>VVEIN-4</t>
-  </si>
-  <si>
-    <t>VVEIN-5</t>
-  </si>
-  <si>
-    <t>VVEIN-6</t>
-  </si>
-  <si>
-    <t>VVEIN-7</t>
-  </si>
-  <si>
     <t>VVAUS</t>
   </si>
   <si>
-    <t>VVAUS-1</t>
-  </si>
-  <si>
-    <t>VVAUS-2</t>
-  </si>
-  <si>
-    <t>VVAUS-3</t>
-  </si>
-  <si>
-    <t>VVAUS-4</t>
-  </si>
-  <si>
-    <t>Position</t>
+    <t>IBEIN1</t>
+  </si>
+  <si>
+    <t>IBEIN2</t>
+  </si>
+  <si>
+    <t>IBEIN3</t>
+  </si>
+  <si>
+    <t>IBEIN4</t>
+  </si>
+  <si>
+    <t>IBEIN5</t>
+  </si>
+  <si>
+    <t>IBEIN6</t>
+  </si>
+  <si>
+    <t>IBEIN7</t>
+  </si>
+  <si>
+    <t>IBEIN8</t>
+  </si>
+  <si>
+    <t>IBEIN9</t>
+  </si>
+  <si>
+    <t>IBAUS1</t>
+  </si>
+  <si>
+    <t>IBAUS2</t>
+  </si>
+  <si>
+    <t>IBAUS3</t>
+  </si>
+  <si>
+    <t>IBAUS4</t>
+  </si>
+  <si>
+    <t>IBAUS5</t>
+  </si>
+  <si>
+    <t>IBAUS6</t>
+  </si>
+  <si>
+    <t>IBAUS7</t>
+  </si>
+  <si>
+    <t>IBAUS8</t>
+  </si>
+  <si>
+    <t>IBAUS9</t>
+  </si>
+  <si>
+    <t>IBAUS10</t>
+  </si>
+  <si>
+    <t>VVEIN1</t>
+  </si>
+  <si>
+    <t>VVEIN2</t>
+  </si>
+  <si>
+    <t>VVEIN3</t>
+  </si>
+  <si>
+    <t>VVEIN4</t>
+  </si>
+  <si>
+    <t>VVEIN5</t>
+  </si>
+  <si>
+    <t>VVEIN6</t>
+  </si>
+  <si>
+    <t>VVEIN7</t>
+  </si>
+  <si>
+    <t>VVAUS1</t>
+  </si>
+  <si>
+    <t>VVAUS2</t>
+  </si>
+  <si>
+    <t>VVAUS3</t>
+  </si>
+  <si>
+    <t>VVAUS4</t>
+  </si>
+  <si>
+    <t>ZBEIN1</t>
+  </si>
+  <si>
+    <t>ZBEIN2</t>
+  </si>
+  <si>
+    <t>ZBEIN3</t>
+  </si>
+  <si>
+    <t>ZBEIN4</t>
+  </si>
+  <si>
+    <t>ZBAUS1</t>
+  </si>
+  <si>
+    <t>ZBAUS2</t>
+  </si>
+  <si>
+    <t>ZBAUS3</t>
+  </si>
+  <si>
+    <t>ZBAUS4</t>
+  </si>
+  <si>
+    <t>ZBAUS5</t>
+  </si>
+  <si>
+    <t>ZBAUS6</t>
+  </si>
+  <si>
+    <t>ZBAUS7</t>
+  </si>
+  <si>
+    <t>ZBAUS8</t>
+  </si>
+  <si>
+    <t>ZBAUS9</t>
+  </si>
+  <si>
+    <t>GBEIN1</t>
+  </si>
+  <si>
+    <t>GBEIN2</t>
+  </si>
+  <si>
+    <t>GBEIN3</t>
+  </si>
+  <si>
+    <t>GBEIN4</t>
+  </si>
+  <si>
+    <t>GBEIN5</t>
+  </si>
+  <si>
+    <t>GBAUS1</t>
+  </si>
+  <si>
+    <t>GBAUS2</t>
+  </si>
+  <si>
+    <t>GBAUS3</t>
+  </si>
+  <si>
+    <t>GBAUS4</t>
+  </si>
+  <si>
+    <t>GBAUS5</t>
+  </si>
+  <si>
+    <t>GBAUS6</t>
+  </si>
+  <si>
+    <t>GBAUS7</t>
+  </si>
+  <si>
+    <t>GBAUS8</t>
+  </si>
+  <si>
+    <t>GBAUS9</t>
+  </si>
+  <si>
+    <t>GBAUS10</t>
+  </si>
+  <si>
+    <t>GBAUS11</t>
+  </si>
+  <si>
+    <t>GBAUS12</t>
+  </si>
+  <si>
+    <t>GBAUS13</t>
   </si>
 </sst>
 </file>
@@ -2992,7 +2989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1033"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A259" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -3029,7 +3026,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>860</v>
+        <v>810</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -8640,13 +8637,13 @@
       </c>
       <c r="F209" s="4" t="str">
         <f>IF(H209="","", _xlfn.XLOOKUP(H209,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G209" s="4">
         <v>0</v>
       </c>
       <c r="H209" s="3" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I209" s="4"/>
     </row>
@@ -8669,13 +8666,13 @@
       </c>
       <c r="F210" s="4" t="str">
         <f>IF(H210="","", _xlfn.XLOOKUP(H210,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-2</v>
+        <v>IBEIN2</v>
       </c>
       <c r="G210" s="4">
         <v>0</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>852</v>
+        <v>802</v>
       </c>
       <c r="I210" s="4"/>
     </row>
@@ -8698,13 +8695,13 @@
       </c>
       <c r="F211" s="4" t="str">
         <f>IF(H211="","", _xlfn.XLOOKUP(H211,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-2</v>
+        <v>IBEIN2</v>
       </c>
       <c r="G211" s="4">
         <v>0</v>
       </c>
       <c r="H211" s="4" t="s">
-        <v>852</v>
+        <v>802</v>
       </c>
       <c r="I211" s="4"/>
     </row>
@@ -8727,13 +8724,13 @@
       </c>
       <c r="F212" s="4" t="str">
         <f>IF(H212="","", _xlfn.XLOOKUP(H212,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-3</v>
+        <v>IBEIN3</v>
       </c>
       <c r="G212" s="4">
         <v>0</v>
       </c>
       <c r="H212" s="4" t="s">
-        <v>853</v>
+        <v>803</v>
       </c>
       <c r="I212" s="4"/>
     </row>
@@ -8756,13 +8753,13 @@
       </c>
       <c r="F213" s="4" t="str">
         <f>IF(H213="","", _xlfn.XLOOKUP(H213,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-3</v>
+        <v>IBEIN3</v>
       </c>
       <c r="G213" s="4">
         <v>0</v>
       </c>
       <c r="H213" s="4" t="s">
-        <v>853</v>
+        <v>803</v>
       </c>
       <c r="I213" s="4"/>
     </row>
@@ -8785,13 +8782,13 @@
       </c>
       <c r="F214" s="4" t="str">
         <f>IF(H214="","", _xlfn.XLOOKUP(H214,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-3</v>
+        <v>IBEIN3</v>
       </c>
       <c r="G214" s="4">
         <v>0</v>
       </c>
       <c r="H214" s="4" t="s">
-        <v>853</v>
+        <v>803</v>
       </c>
       <c r="I214" s="4"/>
     </row>
@@ -8814,13 +8811,13 @@
       </c>
       <c r="F215" s="4" t="str">
         <f>IF(H215="","", _xlfn.XLOOKUP(H215,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-4</v>
+        <v>IBEIN4</v>
       </c>
       <c r="G215" s="4">
         <v>0</v>
       </c>
       <c r="H215" s="4" t="s">
-        <v>854</v>
+        <v>804</v>
       </c>
       <c r="I215" s="4"/>
     </row>
@@ -8843,13 +8840,13 @@
       </c>
       <c r="F216" s="4" t="str">
         <f>IF(H216="","", _xlfn.XLOOKUP(H216,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-4</v>
+        <v>IBEIN4</v>
       </c>
       <c r="G216" s="4">
         <v>0</v>
       </c>
       <c r="H216" s="4" t="s">
-        <v>854</v>
+        <v>804</v>
       </c>
       <c r="I216" s="4"/>
     </row>
@@ -8872,13 +8869,13 @@
       </c>
       <c r="F217" s="4" t="str">
         <f>IF(H217="","", _xlfn.XLOOKUP(H217,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-4</v>
+        <v>IBEIN4</v>
       </c>
       <c r="G217" s="4">
         <v>0</v>
       </c>
       <c r="H217" s="4" t="s">
-        <v>854</v>
+        <v>804</v>
       </c>
       <c r="I217" s="4"/>
     </row>
@@ -8901,13 +8898,13 @@
       </c>
       <c r="F218" s="4" t="str">
         <f>IF(H218="","", _xlfn.XLOOKUP(H218,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-4</v>
+        <v>IBEIN4</v>
       </c>
       <c r="G218" s="4">
         <v>0</v>
       </c>
       <c r="H218" s="4" t="s">
-        <v>854</v>
+        <v>804</v>
       </c>
       <c r="I218" s="4"/>
     </row>
@@ -8930,13 +8927,13 @@
       </c>
       <c r="F219" s="4" t="str">
         <f>IF(H219="","", _xlfn.XLOOKUP(H219,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G219" s="4">
         <v>0</v>
       </c>
       <c r="H219" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I219" s="4"/>
     </row>
@@ -8959,13 +8956,13 @@
       </c>
       <c r="F220" s="4" t="str">
         <f>IF(H220="","", _xlfn.XLOOKUP(H220,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G220" s="4">
         <v>0</v>
       </c>
       <c r="H220" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I220" s="4"/>
     </row>
@@ -8988,13 +8985,13 @@
       </c>
       <c r="F221" s="4" t="str">
         <f>IF(H221="","", _xlfn.XLOOKUP(H221,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G221" s="4">
         <v>0</v>
       </c>
       <c r="H221" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I221" s="4"/>
     </row>
@@ -9017,13 +9014,13 @@
       </c>
       <c r="F222" s="4" t="str">
         <f>IF(H222="","", _xlfn.XLOOKUP(H222,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G222" s="4">
         <v>0</v>
       </c>
       <c r="H222" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I222" s="4"/>
     </row>
@@ -9046,13 +9043,13 @@
       </c>
       <c r="F223" s="4" t="str">
         <f>IF(H223="","", _xlfn.XLOOKUP(H223,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G223" s="4">
         <v>0</v>
       </c>
       <c r="H223" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I223" s="4"/>
     </row>
@@ -9075,13 +9072,13 @@
       </c>
       <c r="F224" s="4" t="str">
         <f>IF(H224="","", _xlfn.XLOOKUP(H224,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G224" s="4">
         <v>0</v>
       </c>
       <c r="H224" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I224" s="4"/>
     </row>
@@ -9104,13 +9101,13 @@
       </c>
       <c r="F225" s="4" t="str">
         <f>IF(H225="","", _xlfn.XLOOKUP(H225,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G225" s="4">
         <v>0</v>
       </c>
       <c r="H225" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I225" s="4"/>
     </row>
@@ -9133,13 +9130,13 @@
       </c>
       <c r="F226" s="4" t="str">
         <f>IF(H226="","", _xlfn.XLOOKUP(H226,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G226" s="4">
         <v>0</v>
       </c>
       <c r="H226" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I226" s="4"/>
     </row>
@@ -9162,13 +9159,13 @@
       </c>
       <c r="F227" s="4" t="str">
         <f>IF(H227="","", _xlfn.XLOOKUP(H227,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBEIN-1</v>
+        <v>IBEIN1</v>
       </c>
       <c r="G227" s="4">
         <v>0</v>
       </c>
       <c r="H227" s="4" t="s">
-        <v>851</v>
+        <v>801</v>
       </c>
       <c r="I227" s="4"/>
     </row>
@@ -9191,13 +9188,13 @@
       </c>
       <c r="F228" s="4" t="str">
         <f>IF(H228="","", _xlfn.XLOOKUP(H228,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-1</v>
+        <v>IBAUS1</v>
       </c>
       <c r="G228" s="4">
         <v>0</v>
       </c>
       <c r="H228" s="4" t="s">
-        <v>855</v>
+        <v>805</v>
       </c>
       <c r="I228" s="4"/>
     </row>
@@ -9220,13 +9217,13 @@
       </c>
       <c r="F229" s="4" t="str">
         <f>IF(H229="","", _xlfn.XLOOKUP(H229,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-1</v>
+        <v>IBAUS1</v>
       </c>
       <c r="G229" s="4">
         <v>0</v>
       </c>
       <c r="H229" s="4" t="s">
-        <v>855</v>
+        <v>805</v>
       </c>
       <c r="I229" s="4"/>
     </row>
@@ -9249,13 +9246,13 @@
       </c>
       <c r="F230" s="4" t="str">
         <f>IF(H230="","", _xlfn.XLOOKUP(H230,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-1</v>
+        <v>IBAUS1</v>
       </c>
       <c r="G230" s="4">
         <v>0</v>
       </c>
       <c r="H230" s="4" t="s">
-        <v>855</v>
+        <v>805</v>
       </c>
       <c r="I230" s="4"/>
     </row>
@@ -9278,13 +9275,13 @@
       </c>
       <c r="F231" s="4" t="str">
         <f>IF(H231="","", _xlfn.XLOOKUP(H231,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G231" s="4">
         <v>0</v>
       </c>
       <c r="H231" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I231" s="4"/>
     </row>
@@ -9307,13 +9304,13 @@
       </c>
       <c r="F232" s="4" t="str">
         <f>IF(H232="","", _xlfn.XLOOKUP(H232,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G232" s="4">
         <v>0</v>
       </c>
       <c r="H232" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I232" s="4"/>
     </row>
@@ -9336,13 +9333,13 @@
       </c>
       <c r="F233" s="4" t="str">
         <f>IF(H233="","", _xlfn.XLOOKUP(H233,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G233" s="4">
         <v>0</v>
       </c>
       <c r="H233" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I233" s="4"/>
     </row>
@@ -9365,13 +9362,13 @@
       </c>
       <c r="F234" s="4" t="str">
         <f>IF(H234="","", _xlfn.XLOOKUP(H234,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G234" s="4">
         <v>0</v>
       </c>
       <c r="H234" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I234" s="4"/>
     </row>
@@ -9394,13 +9391,13 @@
       </c>
       <c r="F235" s="4" t="str">
         <f>IF(H235="","", _xlfn.XLOOKUP(H235,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G235" s="4">
         <v>0</v>
       </c>
       <c r="H235" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I235" s="4"/>
     </row>
@@ -9423,13 +9420,13 @@
       </c>
       <c r="F236" s="4" t="str">
         <f>IF(H236="","", _xlfn.XLOOKUP(H236,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G236" s="4">
         <v>0</v>
       </c>
       <c r="H236" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I236" s="4"/>
     </row>
@@ -9452,13 +9449,13 @@
       </c>
       <c r="F237" s="4" t="str">
         <f>IF(H237="","", _xlfn.XLOOKUP(H237,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G237" s="4">
         <v>0</v>
       </c>
       <c r="H237" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I237" s="4"/>
     </row>
@@ -9481,13 +9478,13 @@
       </c>
       <c r="F238" s="4" t="str">
         <f>IF(H238="","", _xlfn.XLOOKUP(H238,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G238" s="4">
         <v>0</v>
       </c>
       <c r="H238" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I238" s="4"/>
     </row>
@@ -9510,13 +9507,13 @@
       </c>
       <c r="F239" s="4" t="str">
         <f>IF(H239="","", _xlfn.XLOOKUP(H239,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G239" s="4">
         <v>0</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I239" s="4"/>
     </row>
@@ -9539,13 +9536,13 @@
       </c>
       <c r="F240" s="4" t="str">
         <f>IF(H240="","", _xlfn.XLOOKUP(H240,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G240" s="4">
         <v>0</v>
       </c>
       <c r="H240" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I240" s="4"/>
     </row>
@@ -9568,13 +9565,13 @@
       </c>
       <c r="F241" s="4" t="str">
         <f>IF(H241="","", _xlfn.XLOOKUP(H241,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-3</v>
+        <v>IBAUS3</v>
       </c>
       <c r="G241" s="4">
         <v>0</v>
       </c>
       <c r="H241" s="4" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="I241" s="4"/>
     </row>
@@ -9597,13 +9594,13 @@
       </c>
       <c r="F242" s="4" t="str">
         <f>IF(H242="","", _xlfn.XLOOKUP(H242,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-4</v>
+        <v>IBAUS4</v>
       </c>
       <c r="G242" s="4">
         <v>0</v>
       </c>
       <c r="H242" s="4" t="s">
-        <v>858</v>
+        <v>808</v>
       </c>
       <c r="I242" s="4"/>
     </row>
@@ -9626,13 +9623,13 @@
       </c>
       <c r="F243" s="4" t="str">
         <f>IF(H243="","", _xlfn.XLOOKUP(H243,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-4</v>
+        <v>IBAUS4</v>
       </c>
       <c r="G243" s="4">
         <v>0</v>
       </c>
       <c r="H243" s="4" t="s">
-        <v>858</v>
+        <v>808</v>
       </c>
       <c r="I243" s="4"/>
     </row>
@@ -9655,13 +9652,13 @@
       </c>
       <c r="F244" s="4" t="str">
         <f>IF(H244="","", _xlfn.XLOOKUP(H244,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-4</v>
+        <v>IBAUS4</v>
       </c>
       <c r="G244" s="4">
         <v>0</v>
       </c>
       <c r="H244" s="4" t="s">
-        <v>858</v>
+        <v>808</v>
       </c>
       <c r="I244" s="4"/>
     </row>
@@ -9684,13 +9681,13 @@
       </c>
       <c r="F245" s="4" t="str">
         <f>IF(H245="","", _xlfn.XLOOKUP(H245,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-4</v>
+        <v>IBAUS4</v>
       </c>
       <c r="G245" s="4">
         <v>0</v>
       </c>
       <c r="H245" s="4" t="s">
-        <v>858</v>
+        <v>808</v>
       </c>
       <c r="I245" s="4"/>
     </row>
@@ -9713,13 +9710,13 @@
       </c>
       <c r="F246" s="4" t="str">
         <f>IF(H246="","", _xlfn.XLOOKUP(H246,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-4</v>
+        <v>IBAUS4</v>
       </c>
       <c r="G246" s="4">
         <v>0</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>858</v>
+        <v>808</v>
       </c>
       <c r="I246" s="4"/>
     </row>
@@ -9742,13 +9739,13 @@
       </c>
       <c r="F247" s="4" t="str">
         <f>IF(H247="","", _xlfn.XLOOKUP(H247,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-5</v>
+        <v>IBAUS5</v>
       </c>
       <c r="G247" s="4">
         <v>0</v>
       </c>
       <c r="H247" s="4" t="s">
-        <v>859</v>
+        <v>809</v>
       </c>
       <c r="I247" s="4"/>
     </row>
@@ -9771,13 +9768,13 @@
       </c>
       <c r="F248" s="4" t="str">
         <f>IF(H248="","", _xlfn.XLOOKUP(H248,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-5</v>
+        <v>IBAUS5</v>
       </c>
       <c r="G248" s="4">
         <v>0</v>
       </c>
       <c r="H248" s="4" t="s">
-        <v>859</v>
+        <v>809</v>
       </c>
       <c r="I248" s="4"/>
     </row>
@@ -9800,13 +9797,13 @@
       </c>
       <c r="F249" s="4" t="str">
         <f>IF(H249="","", _xlfn.XLOOKUP(H249,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-5</v>
+        <v>IBAUS5</v>
       </c>
       <c r="G249" s="4">
         <v>0</v>
       </c>
       <c r="H249" s="4" t="s">
-        <v>859</v>
+        <v>809</v>
       </c>
       <c r="I249" s="4"/>
     </row>
@@ -9829,13 +9826,13 @@
       </c>
       <c r="F250" s="4" t="str">
         <f>IF(H250="","", _xlfn.XLOOKUP(H250,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G250" s="4">
         <v>0</v>
       </c>
       <c r="H250" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I250" s="4"/>
     </row>
@@ -9858,13 +9855,13 @@
       </c>
       <c r="F251" s="4" t="str">
         <f>IF(H251="","", _xlfn.XLOOKUP(H251,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G251" s="4">
         <v>0</v>
       </c>
       <c r="H251" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I251" s="4"/>
     </row>
@@ -9887,13 +9884,13 @@
       </c>
       <c r="F252" s="4" t="str">
         <f>IF(H252="","", _xlfn.XLOOKUP(H252,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G252" s="4">
         <v>0</v>
       </c>
       <c r="H252" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I252" s="4"/>
     </row>
@@ -9916,13 +9913,13 @@
       </c>
       <c r="F253" s="4" t="str">
         <f>IF(H253="","", _xlfn.XLOOKUP(H253,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G253" s="4">
         <v>0</v>
       </c>
       <c r="H253" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I253" s="4"/>
     </row>
@@ -9945,13 +9942,13 @@
       </c>
       <c r="F254" s="4" t="str">
         <f>IF(H254="","", _xlfn.XLOOKUP(H254,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G254" s="4">
         <v>0</v>
       </c>
       <c r="H254" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I254" s="4"/>
     </row>
@@ -9974,13 +9971,13 @@
       </c>
       <c r="F255" s="4" t="str">
         <f>IF(H255="","", _xlfn.XLOOKUP(H255,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G255" s="4">
         <v>0</v>
       </c>
       <c r="H255" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I255" s="4"/>
     </row>
@@ -10003,13 +10000,13 @@
       </c>
       <c r="F256" s="4" t="str">
         <f>IF(H256="","", _xlfn.XLOOKUP(H256,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G256" s="4">
         <v>0</v>
       </c>
       <c r="H256" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I256" s="4"/>
     </row>
@@ -10032,13 +10029,13 @@
       </c>
       <c r="F257" s="4" t="str">
         <f>IF(H257="","", _xlfn.XLOOKUP(H257,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G257" s="4">
         <v>0</v>
       </c>
       <c r="H257" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I257" s="4"/>
     </row>
@@ -10061,13 +10058,13 @@
       </c>
       <c r="F258" s="4" t="str">
         <f>IF(H258="","", _xlfn.XLOOKUP(H258,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G258" s="4">
         <v>0</v>
       </c>
       <c r="H258" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I258" s="4"/>
     </row>
@@ -10090,13 +10087,13 @@
       </c>
       <c r="F259" s="4" t="str">
         <f>IF(H259="","", _xlfn.XLOOKUP(H259,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G259" s="4">
         <v>0</v>
       </c>
       <c r="H259" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I259" s="4"/>
     </row>
@@ -10119,13 +10116,13 @@
       </c>
       <c r="F260" s="4" t="str">
         <f>IF(H260="","", _xlfn.XLOOKUP(H260,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G260" s="4">
         <v>0</v>
       </c>
       <c r="H260" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I260" s="4"/>
     </row>
@@ -10148,13 +10145,13 @@
       </c>
       <c r="F261" s="4" t="str">
         <f>IF(H261="","", _xlfn.XLOOKUP(H261,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G261" s="4">
         <v>0</v>
       </c>
       <c r="H261" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I261" s="4"/>
     </row>
@@ -10177,13 +10174,13 @@
       </c>
       <c r="F262" s="4" t="str">
         <f>IF(H262="","", _xlfn.XLOOKUP(H262,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G262" s="4">
         <v>0</v>
       </c>
       <c r="H262" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I262" s="4"/>
     </row>
@@ -10206,13 +10203,13 @@
       </c>
       <c r="F263" s="4" t="str">
         <f>IF(H263="","", _xlfn.XLOOKUP(H263,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G263" s="4">
         <v>0</v>
       </c>
       <c r="H263" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I263" s="4"/>
     </row>
@@ -10235,13 +10232,13 @@
       </c>
       <c r="F264" s="4" t="str">
         <f>IF(H264="","", _xlfn.XLOOKUP(H264,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G264" s="4">
         <v>0</v>
       </c>
       <c r="H264" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I264" s="4"/>
     </row>
@@ -10264,13 +10261,13 @@
       </c>
       <c r="F265" s="4" t="str">
         <f>IF(H265="","", _xlfn.XLOOKUP(H265,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G265" s="4">
         <v>0</v>
       </c>
       <c r="H265" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I265" s="4"/>
     </row>
@@ -10293,13 +10290,13 @@
       </c>
       <c r="F266" s="4" t="str">
         <f>IF(H266="","", _xlfn.XLOOKUP(H266,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G266" s="4">
         <v>0</v>
       </c>
       <c r="H266" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I266" s="4"/>
     </row>
@@ -10322,13 +10319,13 @@
       </c>
       <c r="F267" s="4" t="str">
         <f>IF(H267="","", _xlfn.XLOOKUP(H267,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G267" s="4">
         <v>0</v>
       </c>
       <c r="H267" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I267" s="4"/>
     </row>
@@ -10351,13 +10348,13 @@
       </c>
       <c r="F268" s="4" t="str">
         <f>IF(H268="","", _xlfn.XLOOKUP(H268,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G268" s="4">
         <v>0</v>
       </c>
       <c r="H268" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I268" s="4"/>
     </row>
@@ -10380,13 +10377,13 @@
       </c>
       <c r="F269" s="4" t="str">
         <f>IF(H269="","", _xlfn.XLOOKUP(H269,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G269" s="4">
         <v>0</v>
       </c>
       <c r="H269" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I269" s="4"/>
     </row>
@@ -10409,13 +10406,13 @@
       </c>
       <c r="F270" s="4" t="str">
         <f>IF(H270="","", _xlfn.XLOOKUP(H270,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G270" s="4">
         <v>0</v>
       </c>
       <c r="H270" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I270" s="4"/>
     </row>
@@ -10438,13 +10435,13 @@
       </c>
       <c r="F271" s="4" t="str">
         <f>IF(H271="","", _xlfn.XLOOKUP(H271,'EÜR Zuordnung'!B:B,'EÜR Zuordnung'!A:A,""))</f>
-        <v>IBAUS-2</v>
+        <v>IBAUS2</v>
       </c>
       <c r="G271" s="4">
         <v>0</v>
       </c>
       <c r="H271" s="4" t="s">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="I271" s="4"/>
     </row>
@@ -30288,10 +30285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A4D166-79B5-754E-AFAF-3C2785E25EF9}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30299,1731 +30296,1519 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="32.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="2" customWidth="1"/>
-    <col min="4" max="6" width="15.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="2"/>
-    <col min="10" max="10" width="63.33203125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="15.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="63.33203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(H3)," (",E3," - ",F3,")")</f>
+        <v>Gesamt (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D3" s="2" t="str" cm="1">
+        <f t="array" ref="D3">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A3))=A3) * (A:A&lt;&gt;A3)))</f>
+        <v>IBEIN1 + IBEIN2 + IBEIN3 + IBEIN4 + IBEIN5 + IBEIN6 + IBEIN7 + IBEIN8 + IBEIN9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f t="shared" ref="B4:B78" si="0">_xlfn.CONCAT(TRIM(H4)," (",E4," - ",F4,")")</f>
+        <v>Sonstige nicht steuerbare Einnahmen (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E4" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>883</v>
-      </c>
-      <c r="G1" s="6" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Mitgliedsbeiträge (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="H1" s="6" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Aufnahmegebühren (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="J1" s="6" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Zuschüsse (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="B3" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J3)," (",G3," - ",H3,")")</f>
-        <v>Gesamt (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Schenkungen (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="D3" s="2" t="str" cm="1">
-        <f t="array" ref="D3">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A3 &amp; "-", A:A), 0)=1))</f>
-        <v>IBEIN-1 + IBEIN-2 + IBEIN-3 + IBEIN-4 + IBEIN-5 + IBEIN-6 + IBEIN-7 + IBEIN-8 + IBEIN-9</v>
-      </c>
-      <c r="E3" s="2">
-        <v>100</v>
-      </c>
-      <c r="G3" s="2" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Erbschaften/ Vermächtnisse (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>762</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J4)," (",G4," - ",H4,")")</f>
-        <v>Sonstige nicht steuerbare Einnahmen (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E4" s="2">
-        <v>101</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J5)," (",G5," - ",H5,")")</f>
-        <v>Mitgliedsbeiträge (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E5" s="2">
-        <v>102</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J6)," (",G6," - ",H6,")")</f>
-        <v>Aufnahmegebühren (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E6" s="2">
-        <v>103</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J7)," (",G7," - ",H7,")")</f>
-        <v>Zuschüsse (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E7" s="2">
-        <v>104</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>770</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J8)," (",G8," - ",H8,")")</f>
-        <v>Sonstige steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E8" s="2">
-        <v>105</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>772</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J9)," (",G9," - ",H9,")")</f>
-        <v>Schenkungen (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E9" s="2">
-        <v>106</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>774</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J10)," (",G10," - ",H10,")")</f>
-        <v>Erbschaften/ Vermächtnisse (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E10" s="2">
-        <v>107</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>776</v>
+        <v>829</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J11)," (",G11," - ",H11,")")</f>
+        <f t="shared" si="0"/>
         <v>Spenden (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E11" s="2">
-        <v>108</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>762</v>
+        <v>755</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>753</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="J11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gesamt (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D14" s="2" t="str" cm="1">
+        <f t="array" ref="D14">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A14))=A14) * (A:A&lt;&gt;A14)))</f>
+        <v>IBAUS1 + IBAUS2 + IBAUS3 + IBAUS4 + IBAUS5 + IBAUS6 + IBAUS7 + IBAUS8 + IBAUS9 + IBAUS10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Abschreibungen (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Personalkosten (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Reisekosten (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Raumkosten (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gezahlte/hingegebene Spenden (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gesamt (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D26" s="2" t="str" cm="1">
+        <f t="array" ref="D26">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A26))=A26) * (A:A&lt;&gt;A26)))</f>
+        <v>VVEIN1 + VVEIN2 + VVEIN3 + VVEIN4 + VVEIN5 + VVEIN6 + VVEIN7</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige ertragsteuerfreie Einnahmen gemeinnütziger Vereine (gV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Miet- und Pachterträge (gV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Zins- und Kurserträge (gV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Erträge Werbung (gV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige ertragsteuerpflichtige Einnahmen nicht gemeinnütziger Vereine (ngV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="B32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Miet- und Pachterträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Zins- und Kurserträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gesamt (Vermögensverwaltung - Ausgaben)</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D35" s="2" t="str" cm="1">
+        <f t="array" ref="D35">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A35))=A35) * (A:A&lt;&gt;A35)))</f>
+        <v>VVAUS1 + VVAUS2 + VVAUS3 + VVAUS4</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Abschreibungen (Vermögensverwaltung - Ausgaben)</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige Ausgaben (Vermögensverwaltung - Ausgaben)</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Löhne und Gehälter (Vermögensverwaltung - Ausgaben)</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Soziale Abgaben (Vermögensverwaltung - Ausgaben)</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gesamt (Zweckbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D41" s="2" t="str" cm="1">
+        <f t="array" ref="D41">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A41))=A41) * (A:A&lt;&gt;A41)))</f>
+        <v>ZBEIN1 + ZBEIN2 + ZBEIN3 + ZBEIN4</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="B42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Umsatzerlöse (Zweckbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="B43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Bestandsveränderung (Zweckbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="B44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Andere aktivierte Eigenleistungen (Zweckbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige betriebliche Erträge (Zweckbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>778</v>
       </c>
-      <c r="B12" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J12)," (",G12," - ",H12,")")</f>
-        <v>Steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E12" s="2">
-        <v>109</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J12" s="2" t="s">
+      <c r="B47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gesamt (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D47" s="2" t="str" cm="1">
+        <f t="array" ref="D47">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A47))=A47) * (A:A&lt;&gt;A47)))</f>
+        <v>ZBAUS1 + ZBAUS2 + ZBAUS3 + ZBAUS4 + ZBAUS5 + ZBAUS6 + ZBAUS7 + ZBAUS8 + ZBAUS9</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Umsatzerlöse (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="B49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Aufwendungen für bezogene Leistungen (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="B50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Löhne und Gehälter (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>780</v>
       </c>
-      <c r="B14" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J14)," (",G14," - ",H14,")")</f>
-        <v>Gesamt (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D14" s="2" t="str" cm="1">
-        <f t="array" ref="D14">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A14 &amp; "-", A:A), 0)=1))</f>
-        <v>IBAUS-1 + IBAUS-2 + IBAUS-3 + IBAUS-4 + IBAUS-5 + IBAUS-6 + IBAUS-7 + IBAUS-8 + IBAUS-9 + IBAUS-10</v>
-      </c>
-      <c r="E14" s="2">
-        <v>150</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="B15" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J15)," (",G15," - ",H15,")")</f>
-        <v>Abschreibungen (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E15" s="2">
-        <v>151</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="B16" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J16)," (",G16," - ",H16,")")</f>
-        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E16" s="2">
-        <v>152</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="B17" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J17)," (",G17," - ",H17,")")</f>
-        <v>Personalkosten (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E17" s="2">
-        <v>153</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="B18" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J18)," (",G18," - ",H18,")")</f>
-        <v>Reisekosten (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E18" s="2">
-        <v>154</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>752</v>
-      </c>
-      <c r="B19" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J19)," (",G19," - ",H19,")")</f>
-        <v>Raumkosten (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E19" s="2">
-        <v>155</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="B20" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J20)," (",G20," - ",H20,")")</f>
-        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E20" s="2">
-        <v>156</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>787</v>
-      </c>
-      <c r="B21" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J21)," (",G21," - ",H21,")")</f>
-        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E21" s="2">
-        <v>157</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="B22" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J22)," (",G22," - ",H22,")")</f>
-        <v>Gezahlte/hingegebene Spenden (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E22" s="2">
-        <v>158</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>791</v>
-      </c>
-      <c r="B23" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J23)," (",G23," - ",H23,")")</f>
-        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E23" s="2">
-        <v>159</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>792</v>
-      </c>
-      <c r="B24" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J24)," (",G24," - ",H24,")")</f>
-        <v>Nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E24" s="2">
-        <v>160</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>870</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J26)," (",G26," - ",H26,")")</f>
-        <v>Gesamt (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D26" s="2" t="str" cm="1">
-        <f t="array" ref="D26">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A26 &amp; "-", A:A), 0)=1))</f>
-        <v>VVEIN-1 + VVEIN-2 + VVEIN-3 + VVEIN-4 + VVEIN-5 + VVEIN-6 + VVEIN-7</v>
-      </c>
-      <c r="E26" s="2">
-        <v>200</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>871</v>
-      </c>
-      <c r="B27" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J27)," (",G27," - ",H27,")")</f>
-        <v>Sonstige ertragsteuerfreie Einnahmen gemeinnütziger Vereine (gV) (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E27" s="2">
-        <v>201</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>872</v>
-      </c>
-      <c r="B28" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J28)," (",G28," - ",H28,")")</f>
-        <v>Miet- und Pachterträge (gV) (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E28" s="2">
-        <v>202</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>873</v>
-      </c>
-      <c r="B29" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J29)," (",G29," - ",H29,")")</f>
-        <v>Zins- und Kurserträge (gV) (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E29" s="2">
-        <v>203</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>874</v>
-      </c>
-      <c r="B30" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J30)," (",G30," - ",H30,")")</f>
-        <v>Erträge Werbung (gV) (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E30" s="2">
-        <v>204</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>875</v>
-      </c>
-      <c r="B31" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J31)," (",G31," - ",H31,")")</f>
-        <v>Sonstige ertragsteuerpflichtige Einnahmen nicht gemeinnütziger Vereine (ngV) (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E31" s="2">
-        <v>205</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>876</v>
-      </c>
-      <c r="B32" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J32)," (",G32," - ",H32,")")</f>
-        <v>Miet- und Pachterträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E32" s="2">
-        <v>206</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>877</v>
-      </c>
-      <c r="B33" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J33)," (",G33," - ",H33,")")</f>
-        <v>Zins- und Kurserträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E33" s="2">
-        <v>207</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>878</v>
-      </c>
-      <c r="B35" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J35)," (",G35," - ",H35,")")</f>
-        <v>Gesamt (Vermögensverwaltung - Ausgaben)</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D35" s="2" t="str" cm="1">
-        <f t="array" ref="D35">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A35 &amp; "-", A:A), 0)=1))</f>
-        <v>VVAUS-1 + VVAUS-2 + VVAUS-3 + VVAUS-4</v>
-      </c>
-      <c r="E35" s="2">
-        <v>250</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>879</v>
-      </c>
-      <c r="B36" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J36)," (",G36," - ",H36,")")</f>
-        <v>Abschreibungen (Vermögensverwaltung - Ausgaben)</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E36" s="2">
-        <v>251</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>880</v>
-      </c>
-      <c r="B37" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J37)," (",G37," - ",H37,")")</f>
-        <v>Sonstige Ausgaben (Vermögensverwaltung - Ausgaben)</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E37" s="2">
-        <v>252</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>881</v>
-      </c>
-      <c r="B38" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J38)," (",G38," - ",H38,")")</f>
-        <v>Löhne und Gehälter (Vermögensverwaltung - Ausgaben)</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E38" s="2">
-        <v>253</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>882</v>
-      </c>
-      <c r="B39" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J39)," (",G39," - ",H39,")")</f>
-        <v>Soziale Abgaben (Vermögensverwaltung - Ausgaben)</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E39" s="2">
-        <v>254</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>794</v>
-      </c>
-      <c r="B41" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J41)," (",G41," - ",H41,")")</f>
-        <v>Gesamt (Zweckbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D41" s="2" t="str" cm="1">
-        <f t="array" ref="D41">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A41 &amp; "-", A:A), 0)=1))</f>
-        <v>ZBEIN-1 + ZBEIN-2 + ZBEIN-3 + ZBEIN-4</v>
-      </c>
-      <c r="E41" s="2">
-        <v>300</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>796</v>
-      </c>
-      <c r="B42" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J42)," (",G42," - ",H42,")")</f>
-        <v>Umsatzerlöse (Zweckbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E42" s="2">
-        <v>301</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>797</v>
-      </c>
-      <c r="B43" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J43)," (",G43," - ",H43,")")</f>
-        <v>Bestandsveränderung (Zweckbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E43" s="2">
-        <v>302</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>798</v>
-      </c>
-      <c r="B44" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J44)," (",G44," - ",H44,")")</f>
-        <v>Andere aktivierte Eigenleistungen (Zweckbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E44" s="2">
-        <v>303</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>800</v>
-      </c>
-      <c r="B45" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J45)," (",G45," - ",H45,")")</f>
-        <v>Sonstige betriebliche Erträge (Zweckbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E45" s="2">
-        <v>304</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>801</v>
-      </c>
-      <c r="B47" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J47)," (",G47," - ",H47,")")</f>
-        <v>Gesamt (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D47" s="2" t="str" cm="1">
-        <f t="array" ref="D47">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A47 &amp; "-", A:A), 0)=1))</f>
-        <v>ZBAUS-1 + ZBAUS-2 + ZBAUS-3 + ZBAUS-4 + ZBAUS-5 + ZBAUS-6 + ZBAUS-7 + ZBAUS-8 + ZBAUS-9</v>
-      </c>
-      <c r="E47" s="2">
-        <v>350</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>802</v>
-      </c>
-      <c r="B48" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J48)," (",G48," - ",H48,")")</f>
-        <v>Umsatzerlöse (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E48" s="2">
-        <v>351</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>803</v>
-      </c>
-      <c r="B49" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J49)," (",G49," - ",H49,")")</f>
-        <v>Aufwendungen für bezogene Leistungen (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E49" s="2">
-        <v>352</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>805</v>
-      </c>
-      <c r="B50" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J50)," (",G50," - ",H50,")")</f>
-        <v>Löhne und Gehälter (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E50" s="2">
-        <v>353</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>807</v>
+        <v>859</v>
       </c>
       <c r="B51" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J51)," (",G51," - ",H51,")")</f>
+        <f t="shared" si="0"/>
         <v>Soziale Abgaben (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E51" s="2">
-        <v>354</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>795</v>
+        <v>755</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>766</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>781</v>
       </c>
-      <c r="J51" s="2" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>809</v>
+        <v>860</v>
       </c>
       <c r="B52" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J52)," (",G52," - ",H52,")")</f>
+        <f t="shared" si="0"/>
         <v>Immaterielle Vermögensgegenstände und Sachanlagen (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E52" s="2">
-        <v>355</v>
-      </c>
-      <c r="G52" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="B53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Umlaufvermögen, unüblich hoch (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="B54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige betriebliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Zinsen und ähnliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="B56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige Steuern (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="B58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gesamt (Geschäftsbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D58" s="2" t="str" cm="1">
+        <f t="array" ref="D58">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A58))=A58) * (A:A&lt;&gt;A58)))</f>
+        <v>GBEIN1 + GBEIN2 + GBEIN3 + GBEIN4 + GBEIN5</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Umsatzerlöse (Geschäftsbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="B60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige betriebliche Erträge (Geschäftsbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Bestandsveränderungen (Geschäftsbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="B62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Andere aktivierte Eigenleistungen (Geschäftsbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="B63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige Zinsen und ähnliche Einnahmen (Geschäftsbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="B65" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Gesamt (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D65" s="2" t="str" cm="1">
+        <f t="array" ref="D65">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A65))=A65) * (A:A&lt;&gt;A65)))</f>
+        <v>GBAUS1 + GBAUS2 + GBAUS3 + GBAUS4 + GBAUS5 + GBAUS6 + GBAUS7 + GBAUS8 + GBAUS9 + GBAUS10 + GBAUS11 + GBAUS12 + GBAUS13</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="B66" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Ausgaben für Roh-, Hilfs- und Betriebsstoffe und für bezogene Waren (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B67" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige betriebliche Aufwendungen (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B68" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Aufwendungen für bezogene Leistungen (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="B69" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Löhne und Gehälter (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="B70" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Soziale Abgaben (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="B71" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Immaterielle Vermögensgegenstände und Sachanlagen (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H71" s="2" t="s">
         <v>795</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="B53" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J53)," (",G53," - ",H53,")")</f>
-        <v>Umlaufvermögen, unüblich hoch (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E53" s="2">
-        <v>356</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="B54" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J54)," (",G54," - ",H54,")")</f>
-        <v>Sonstige betriebliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E54" s="2">
-        <v>357</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>815</v>
-      </c>
-      <c r="B55" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J55)," (",G55," - ",H55,")")</f>
-        <v>Zinsen und ähnliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E55" s="2">
-        <v>358</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>817</v>
-      </c>
-      <c r="B56" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J56)," (",G56," - ",H56,")")</f>
-        <v>Sonstige Steuern (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E56" s="2">
-        <v>359</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>819</v>
-      </c>
-      <c r="B58" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J58)," (",G58," - ",H58,")")</f>
-        <v>Gesamt (Geschäftsbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D58" s="2" t="str" cm="1">
-        <f t="array" ref="D58">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A58 &amp; "-", A:A), 0)=1))</f>
-        <v>GBEIN-1 + GBEIN-2 + GBEIN-3 + GBEIN-4 + GBEIN-5</v>
-      </c>
-      <c r="E58" s="2">
-        <v>400</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="B59" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J59)," (",G59," - ",H59,")")</f>
-        <v>Umsatzerlöse (Geschäftsbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E59" s="2">
-        <v>401</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>823</v>
-      </c>
-      <c r="B60" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J60)," (",G60," - ",H60,")")</f>
-        <v>Sonstige betriebliche Erträge (Geschäftsbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E60" s="2">
-        <v>402</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>825</v>
-      </c>
-      <c r="B61" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J61)," (",G61," - ",H61,")")</f>
-        <v>Bestandsveränderungen (Geschäftsbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E61" s="2">
-        <v>403</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="B62" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J62)," (",G62," - ",H62,")")</f>
-        <v>Andere aktivierte Eigenleistungen (Geschäftsbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E62" s="2">
-        <v>404</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J62" s="2" t="s">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B72" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Umlaufvermögen, unüblich hoch (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="B73" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Erträge aus Beteiligungen (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="B74" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Erträge aus anderen Wertpapieren (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="B75" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonstige Zinsen und ähnliche Erträge (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B76" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Abschreibungen auf Finanzanlagen (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>827</v>
-      </c>
-      <c r="B63" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J63)," (",G63," - ",H63,")")</f>
-        <v>Sonstige Zinsen und ähnliche Einnahmen (Geschäftsbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E63" s="2">
-        <v>405</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>829</v>
-      </c>
-      <c r="B65" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J65)," (",G65," - ",H65,")")</f>
-        <v>Gesamt (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D65" s="2" t="str" cm="1">
-        <f t="array" ref="D65">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, IFERROR(SEARCH(A65 &amp; "-", A:A), 0)=1))</f>
-        <v>GBAUS-1 + GBAUS-2 + GBAUS-3 + GBAUS-4 + GBAUS-5 + GBAUS-6 + GBAUS-7 + GBAUS-8 + GBAUS-9 + GBAUS-10 + GBAUS-11 + GBAUS-12 + GBAUS-13</v>
-      </c>
-      <c r="E65" s="2">
-        <v>450</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>830</v>
-      </c>
-      <c r="B66" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J66)," (",G66," - ",H66,")")</f>
-        <v>Ausgaben für Roh-, Hilfs- und Betriebsstoffe und für bezogene Waren (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E66" s="2">
-        <v>451</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>832</v>
-      </c>
-      <c r="B67" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J67)," (",G67," - ",H67,")")</f>
-        <v>Sonstige betriebliche Aufwendungen (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E67" s="2">
-        <v>452</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>833</v>
-      </c>
-      <c r="B68" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J68)," (",G68," - ",H68,")")</f>
-        <v>Aufwendungen für bezogene Leistungen (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E68" s="2">
-        <v>453</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>834</v>
-      </c>
-      <c r="B69" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J69)," (",G69," - ",H69,")")</f>
-        <v>Löhne und Gehälter (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E69" s="2">
-        <v>454</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>835</v>
-      </c>
-      <c r="B70" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J70)," (",G70," - ",H70,")")</f>
-        <v>Soziale Abgaben (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E70" s="2">
-        <v>455</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>837</v>
-      </c>
-      <c r="B71" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J71)," (",G71," - ",H71,")")</f>
-        <v>Immaterielle Vermögensgegenstände und Sachanlagen (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E71" s="2">
-        <v>456</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>839</v>
-      </c>
-      <c r="B72" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J72)," (",G72," - ",H72,")")</f>
-        <v>Umlaufvermögen, unüblich hoch (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E72" s="2">
-        <v>457</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>840</v>
-      </c>
-      <c r="B73" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J73)," (",G73," - ",H73,")")</f>
-        <v>Erträge aus Beteiligungen (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E73" s="2">
-        <v>458</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="B74" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J74)," (",G74," - ",H74,")")</f>
-        <v>Erträge aus anderen Wertpapieren (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E74" s="2">
-        <v>459</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="B75" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J75)," (",G75," - ",H75,")")</f>
-        <v>Sonstige Zinsen und ähnliche Erträge (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E75" s="2">
-        <v>460</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="B76" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J76)," (",G76," - ",H76,")")</f>
-        <v>Abschreibungen auf Finanzanlagen (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E76" s="2">
-        <v>461</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>848</v>
+        <v>881</v>
       </c>
       <c r="B77" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J77)," (",G77," - ",H77,")")</f>
+        <f t="shared" si="0"/>
         <v>Zinsen und ähnliche Aufwendungen (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E77" s="2">
-        <v>462</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>820</v>
+        <v>755</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>766</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>849</v>
+        <v>882</v>
       </c>
       <c r="B78" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(J78)," (",G78," - ",H78,")")</f>
+        <f t="shared" si="0"/>
         <v>Sonstige Steuern (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E78" s="2">
-        <v>463</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>820</v>
+        <v>755</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>766</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="J78" s="2" t="s">
-        <v>818</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix für Fehler bei berechneten Kuntengruppen
</commit_message>
<xml_diff>
--- a/dolibarr-skr49 EUeR.xlsx
+++ b/dolibarr-skr49 EUeR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannes/Documents/Programming/Innwerk/dolibarr-kontenplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BBE6EC-104B-8F43-BD57-24E4D4EBA80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424F8D3B-9C35-384D-89EC-1A5784855CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKR49" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3519" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3520" uniqueCount="884">
   <si>
     <t>Kontenplan</t>
   </si>
@@ -2705,6 +2705,9 @@
   </si>
   <si>
     <t>GBAUS13</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
@@ -30285,10 +30288,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A4D166-79B5-754E-AFAF-3C2785E25EF9}">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30296,15 +30299,14 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="32.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="2"/>
-    <col min="8" max="8" width="63.33203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="6" width="15.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="63.33203125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>744</v>
       </c>
@@ -30318,1497 +30320,1704 @@
         <v>746</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>747</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>748</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>750</v>
+        <v>822</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>_xlfn.CONCAT(TRIM(H3)," (",E3," - ",F3,")")</f>
-        <v>Gesamt (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I3)," (",G3," - ",H3,")")</f>
+        <v>Sonstige nicht steuerbare Einnahmen (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D3" s="2" t="str" cm="1">
-        <f t="array" ref="D3">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A3))=A3) * (A:A&lt;&gt;A3)))</f>
-        <v>IBEIN1 + IBEIN2 + IBEIN3 + IBEIN4 + IBEIN5 + IBEIN6 + IBEIN7 + IBEIN8 + IBEIN9</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f t="shared" ref="B4:B78" si="0">_xlfn.CONCAT(TRIM(H4)," (",E4," - ",F4,")")</f>
-        <v>Sonstige nicht steuerbare Einnahmen (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I4)," (",G4," - ",H4,")")</f>
+        <v>Mitgliedsbeiträge (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2">
+        <v>101</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Mitgliedsbeiträge (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I5)," (",G5," - ",H5,")")</f>
+        <v>Aufnahmegebühren (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2">
+        <v>102</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Aufnahmegebühren (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I6)," (",G6," - ",H6,")")</f>
+        <v>Zuschüsse (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2">
+        <v>103</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Zuschüsse (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I7)," (",G7," - ",H7,")")</f>
+        <v>Sonstige steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2">
+        <v>104</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I8)," (",G8," - ",H8,")")</f>
+        <v>Schenkungen (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2">
+        <v>105</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Schenkungen (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I9)," (",G9," - ",H9,")")</f>
+        <v>Erbschaften/ Vermächtnisse (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2">
+        <v>106</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Erbschaften/ Vermächtnisse (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I10)," (",G10," - ",H10,")")</f>
+        <v>Spenden (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2">
+        <v>107</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Spenden (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I11)," (",G11," - ",H11,")")</f>
+        <v>Steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2">
+        <v>108</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>830</v>
+        <v>750</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Steuerneutrale Einnahmen (Ideeler Bereich - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I12)," (",G12," - ",H12,")")</f>
+        <v>Gesamt (Ideeler Bereich - Einnahmen)</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D12" s="2" t="str" cm="1">
+        <f t="array" ref="D12">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A12))=A12) * (A:A&lt;&gt;A12)))</f>
+        <v>IBEIN1 + IBEIN2 + IBEIN3 + IBEIN4 + IBEIN5 + IBEIN6 + IBEIN7 + IBEIN8 + IBEIN9</v>
+      </c>
+      <c r="F12" s="2">
+        <v>149</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(I14)," (",G14," - ",H14,")")</f>
+        <v>Abschreibungen (Ideeler Bereich - Ausgaben)</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F14" s="2">
+        <v>150</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gesamt (Ideeler Bereich - Ausgaben)</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D14" s="2" t="str" cm="1">
-        <f t="array" ref="D14">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A14))=A14) * (A:A&lt;&gt;A14)))</f>
-        <v>IBAUS1 + IBAUS2 + IBAUS3 + IBAUS4 + IBAUS5 + IBAUS6 + IBAUS7 + IBAUS8 + IBAUS9 + IBAUS10</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>752</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Abschreibungen (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I15)," (",G15," - ",H15,")")</f>
+        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2">
+        <v>151</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I16)," (",G16," - ",H16,")")</f>
+        <v>Personalkosten (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2">
+        <v>152</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Personalkosten (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I17)," (",G17," - ",H17,")")</f>
+        <v>Reisekosten (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2">
+        <v>153</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="2" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Reisekosten (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I18)," (",G18," - ",H18,")")</f>
+        <v>Raumkosten (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2">
+        <v>154</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Raumkosten (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I19)," (",G19," - ",H19,")")</f>
+        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2">
+        <v>155</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Übrige Ausgaben (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I20)," (",G20," - ",H20,")")</f>
+        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2">
+        <v>156</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I21)," (",G21," - ",H21,")")</f>
+        <v>Gezahlte/hingegebene Spenden (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2">
+        <v>157</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gezahlte/hingegebene Spenden (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I22)," (",G22," - ",H22,")")</f>
+        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2">
+        <v>158</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I23)," (",G23," - ",H23,")")</f>
+        <v>Nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2">
+        <v>159</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>840</v>
+        <v>765</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Nicht abziehbare Ausgaben (Ideeler Bereich - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I24)," (",G24," - ",H24,")")</f>
+        <v>Gesamt (Ideeler Bereich - Ausgaben)</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D24" s="2" t="str" cm="1">
+        <f t="array" ref="D24">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A24))=A24) * (A:A&lt;&gt;A24)))</f>
+        <v>IBAUS1 + IBAUS2 + IBAUS3 + IBAUS4 + IBAUS5 + IBAUS6 + IBAUS7 + IBAUS8 + IBAUS9 + IBAUS10</v>
+      </c>
+      <c r="F24" s="2">
+        <v>199</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(I26)," (",G26," - ",H26,")")</f>
+        <v>Sonstige ertragsteuerfreie Einnahmen gemeinnütziger Vereine (gV) (Vermögensverwaltung - Einnahmen)</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>752</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gesamt (Vermögensverwaltung - Einnahmen)</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D26" s="2" t="str" cm="1">
-        <f t="array" ref="D26">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A26))=A26) * (A:A&lt;&gt;A26)))</f>
-        <v>VVEIN1 + VVEIN2 + VVEIN3 + VVEIN4 + VVEIN5 + VVEIN6 + VVEIN7</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2">
+        <v>200</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="2" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige ertragsteuerfreie Einnahmen gemeinnütziger Vereine (gV) (Vermögensverwaltung - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I27)," (",G27," - ",H27,")")</f>
+        <v>Miet- und Pachterträge (gV) (Vermögensverwaltung - Einnahmen)</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2">
+        <v>201</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="2" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Miet- und Pachterträge (gV) (Vermögensverwaltung - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I28)," (",G28," - ",H28,")")</f>
+        <v>Zins- und Kurserträge (gV) (Vermögensverwaltung - Einnahmen)</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2">
+        <v>202</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="2" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Zins- und Kurserträge (gV) (Vermögensverwaltung - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I29)," (",G29," - ",H29,")")</f>
+        <v>Erträge Werbung (gV) (Vermögensverwaltung - Einnahmen)</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2">
+        <v>203</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="2" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Erträge Werbung (gV) (Vermögensverwaltung - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I30)," (",G30," - ",H30,")")</f>
+        <v>Sonstige ertragsteuerpflichtige Einnahmen nicht gemeinnütziger Vereine (ngV) (Vermögensverwaltung - Einnahmen)</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2">
+        <v>204</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="2" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige ertragsteuerpflichtige Einnahmen nicht gemeinnütziger Vereine (ngV) (Vermögensverwaltung - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I31)," (",G31," - ",H31,")")</f>
+        <v>Miet- und Pachterträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2">
+        <v>205</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="2" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Miet- und Pachterträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I32)," (",G32," - ",H32,")")</f>
+        <v>Zins- und Kurserträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2">
+        <v>206</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="2" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>847</v>
+        <v>820</v>
       </c>
       <c r="B33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Zins- und Kurserträge (ngV) (Vermögensverwaltung - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I33)," (",G33," - ",H33,")")</f>
+        <v>Gesamt (Vermögensverwaltung - Einnahmen)</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D33" s="2" t="str" cm="1">
+        <f t="array" ref="D33">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A33))=A33) * (A:A&lt;&gt;A33)))</f>
+        <v>VVEIN1 + VVEIN2 + VVEIN3 + VVEIN4 + VVEIN5 + VVEIN6 + VVEIN7</v>
+      </c>
+      <c r="F33" s="2">
+        <v>249</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(I35)," (",G35," - ",H35,")")</f>
+        <v>Abschreibungen (Vermögensverwaltung - Ausgaben)</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F35" s="2">
+        <v>250</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="B35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gesamt (Vermögensverwaltung - Ausgaben)</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D35" s="2" t="str" cm="1">
-        <f t="array" ref="D35">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A35))=A35) * (A:A&lt;&gt;A35)))</f>
-        <v>VVAUS1 + VVAUS2 + VVAUS3 + VVAUS4</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Abschreibungen (Vermögensverwaltung - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I36)," (",G36," - ",H36,")")</f>
+        <v>Sonstige Ausgaben (Vermögensverwaltung - Ausgaben)</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2">
+        <v>251</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige Ausgaben (Vermögensverwaltung - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I37)," (",G37," - ",H37,")")</f>
+        <v>Löhne und Gehälter (Vermögensverwaltung - Ausgaben)</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2">
+        <v>252</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Löhne und Gehälter (Vermögensverwaltung - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I38)," (",G38," - ",H38,")")</f>
+        <v>Soziale Abgaben (Vermögensverwaltung - Ausgaben)</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2">
+        <v>253</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>851</v>
+        <v>821</v>
       </c>
       <c r="B39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Soziale Abgaben (Vermögensverwaltung - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I39)," (",G39," - ",H39,")")</f>
+        <v>Gesamt (Vermögensverwaltung - Ausgaben)</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D39" s="2" t="str" cm="1">
+        <f t="array" ref="D39">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A39))=A39) * (A:A&lt;&gt;A39)))</f>
+        <v>VVAUS1 + VVAUS2 + VVAUS3 + VVAUS4</v>
+      </c>
+      <c r="F39" s="2">
+        <v>299</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(I41)," (",G41," - ",H41,")")</f>
+        <v>Umsatzerlöse (Zweckbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>775</v>
-      </c>
-      <c r="B41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gesamt (Zweckbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D41" s="2" t="str" cm="1">
-        <f t="array" ref="D41">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A41))=A41) * (A:A&lt;&gt;A41)))</f>
-        <v>ZBEIN1 + ZBEIN2 + ZBEIN3 + ZBEIN4</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2">
+        <v>300</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Umsatzerlöse (Zweckbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I42)," (",G42," - ",H42,")")</f>
+        <v>Bestandsveränderung (Zweckbetrieb - Einnahmen)</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2">
+        <v>301</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Bestandsveränderung (Zweckbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I43)," (",G43," - ",H43,")")</f>
+        <v>Andere aktivierte Eigenleistungen (Zweckbetrieb - Einnahmen)</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2">
+        <v>302</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B44" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Andere aktivierte Eigenleistungen (Zweckbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I44)," (",G44," - ",H44,")")</f>
+        <v>Sonstige betriebliche Erträge (Zweckbetrieb - Einnahmen)</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2">
+        <v>303</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>855</v>
+        <v>775</v>
       </c>
       <c r="B45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige betriebliche Erträge (Zweckbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I45)," (",G45," - ",H45,")")</f>
+        <v>Gesamt (Zweckbetrieb - Einnahmen)</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D45" s="2" t="str" cm="1">
+        <f t="array" ref="D45">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A45))=A45) * (A:A&lt;&gt;A45)))</f>
+        <v>ZBEIN1 + ZBEIN2 + ZBEIN3 + ZBEIN4</v>
+      </c>
+      <c r="F45" s="2">
+        <v>349</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B47" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(I47)," (",G47," - ",H47,")")</f>
+        <v>Umsatzerlöse (Zweckbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F47" s="2">
+        <v>350</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="B47" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gesamt (Zweckbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D47" s="2" t="str" cm="1">
-        <f t="array" ref="D47">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A47))=A47) * (A:A&lt;&gt;A47)))</f>
-        <v>ZBAUS1 + ZBAUS2 + ZBAUS3 + ZBAUS4 + ZBAUS5 + ZBAUS6 + ZBAUS7 + ZBAUS8 + ZBAUS9</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>776</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B48" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Umsatzerlöse (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I48)," (",G48," - ",H48,")")</f>
+        <v>Aufwendungen für bezogene Leistungen (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="2">
+        <v>351</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" s="2" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B49" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Aufwendungen für bezogene Leistungen (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I49)," (",G49," - ",H49,")")</f>
+        <v>Löhne und Gehälter (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2">
+        <v>352</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B50" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Löhne und Gehälter (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I50)," (",G50," - ",H50,")")</f>
+        <v>Soziale Abgaben (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2">
+        <v>353</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" s="2" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B51" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Soziale Abgaben (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I51)," (",G51," - ",H51,")")</f>
+        <v>Immaterielle Vermögensgegenstände und Sachanlagen (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2">
+        <v>354</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" s="2" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B52" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Immaterielle Vermögensgegenstände und Sachanlagen (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I52)," (",G52," - ",H52,")")</f>
+        <v>Umlaufvermögen, unüblich hoch (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2">
+        <v>355</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B53" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Umlaufvermögen, unüblich hoch (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I53)," (",G53," - ",H53,")")</f>
+        <v>Sonstige betriebliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2">
+        <v>356</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B54" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige betriebliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I54)," (",G54," - ",H54,")")</f>
+        <v>Zinsen und ähnliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2">
+        <v>357</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H54" s="2" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B55" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Zinsen und ähnliche Aufwendungen (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I55)," (",G55," - ",H55,")")</f>
+        <v>Sonstige Steuern (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2">
+        <v>358</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>864</v>
+        <v>778</v>
       </c>
       <c r="B56" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige Steuern (Zweckbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I56)," (",G56," - ",H56,")")</f>
+        <v>Gesamt (Zweckbetrieb - Ausgaben)</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D56" s="2" t="str" cm="1">
+        <f t="array" ref="D56">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A56))=A56) * (A:A&lt;&gt;A56)))</f>
+        <v>ZBAUS1 + ZBAUS2 + ZBAUS3 + ZBAUS4 + ZBAUS5 + ZBAUS6 + ZBAUS7 + ZBAUS8 + ZBAUS9</v>
+      </c>
+      <c r="F56" s="2">
+        <v>399</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B58" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(I58)," (",G58," - ",H58,")")</f>
+        <v>Umsatzerlöse (Geschäftsbetrieb - Einnahmen)</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>776</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>787</v>
-      </c>
-      <c r="B58" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gesamt (Geschäftsbetrieb - Einnahmen)</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D58" s="2" t="str" cm="1">
-        <f t="array" ref="D58">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A58))=A58) * (A:A&lt;&gt;A58)))</f>
-        <v>GBEIN1 + GBEIN2 + GBEIN3 + GBEIN4 + GBEIN5</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2">
+        <v>400</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B59" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Umsatzerlöse (Geschäftsbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I59)," (",G59," - ",H59,")")</f>
+        <v>Sonstige betriebliche Erträge (Geschäftsbetrieb - Einnahmen)</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2">
+        <v>401</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H59" s="2" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B60" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige betriebliche Erträge (Geschäftsbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I60)," (",G60," - ",H60,")")</f>
+        <v>Bestandsveränderungen (Geschäftsbetrieb - Einnahmen)</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2">
+        <v>402</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="2" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B61" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Bestandsveränderungen (Geschäftsbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I61)," (",G61," - ",H61,")")</f>
+        <v>Andere aktivierte Eigenleistungen (Geschäftsbetrieb - Einnahmen)</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="2">
+        <v>403</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="H61" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B62" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Andere aktivierte Eigenleistungen (Geschäftsbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I62)," (",G62," - ",H62,")")</f>
+        <v>Sonstige Zinsen und ähnliche Einnahmen (Geschäftsbetrieb - Einnahmen)</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="2">
+        <v>404</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>869</v>
+        <v>787</v>
       </c>
       <c r="B63" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige Zinsen und ähnliche Einnahmen (Geschäftsbetrieb - Einnahmen)</v>
+        <f>_xlfn.CONCAT(TRIM(I63)," (",G63," - ",H63,")")</f>
+        <v>Gesamt (Geschäftsbetrieb - Einnahmen)</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D63" s="2" t="str" cm="1">
+        <f t="array" ref="D63">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A63))=A63) * (A:A&lt;&gt;A63)))</f>
+        <v>GBEIN1 + GBEIN2 + GBEIN3 + GBEIN4 + GBEIN5</v>
+      </c>
+      <c r="F63" s="2">
+        <v>449</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="B65" s="2" t="str">
+        <f>_xlfn.CONCAT(TRIM(I65)," (",G65," - ",H65,")")</f>
+        <v>Ausgaben für Roh-, Hilfs- und Betriebsstoffe und für bezogene Waren (Geschäftsbetrieb - Ausgaben)</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F65" s="2">
+        <v>450</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>792</v>
-      </c>
-      <c r="B65" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Gesamt (Geschäftsbetrieb - Ausgaben)</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D65" s="2" t="str" cm="1">
-        <f t="array" ref="D65">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A65))=A65) * (A:A&lt;&gt;A65)))</f>
-        <v>GBAUS1 + GBAUS2 + GBAUS3 + GBAUS4 + GBAUS5 + GBAUS6 + GBAUS7 + GBAUS8 + GBAUS9 + GBAUS10 + GBAUS11 + GBAUS12 + GBAUS13</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>788</v>
-      </c>
-      <c r="F65" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Ausgaben für Roh-, Hilfs- und Betriebsstoffe und für bezogene Waren (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I66)," (",G66," - ",H66,")")</f>
+        <v>Sonstige betriebliche Aufwendungen (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2">
+        <v>451</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H66" s="2" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B67" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige betriebliche Aufwendungen (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I67)," (",G67," - ",H67,")")</f>
+        <v>Aufwendungen für bezogene Leistungen (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2">
+        <v>452</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="H67" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="2" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B68" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Aufwendungen für bezogene Leistungen (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I68)," (",G68," - ",H68,")")</f>
+        <v>Löhne und Gehälter (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="F68" s="2">
+        <v>453</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="H68" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H68" s="2" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B69" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Löhne und Gehälter (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I69)," (",G69," - ",H69,")")</f>
+        <v>Soziale Abgaben (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="2">
+        <v>454</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B70" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Soziale Abgaben (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I70)," (",G70," - ",H70,")")</f>
+        <v>Immaterielle Vermögensgegenstände und Sachanlagen (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="2">
+        <v>455</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H70" s="2" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B71" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Immaterielle Vermögensgegenstände und Sachanlagen (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I71)," (",G71," - ",H71,")")</f>
+        <v>Umlaufvermögen, unüblich hoch (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2">
+        <v>456</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="H71" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H71" s="2" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B72" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Umlaufvermögen, unüblich hoch (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I72)," (",G72," - ",H72,")")</f>
+        <v>Erträge aus Beteiligungen (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="2">
+        <v>457</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="H72" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" s="2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B73" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Erträge aus Beteiligungen (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I73)," (",G73," - ",H73,")")</f>
+        <v>Erträge aus anderen Wertpapieren (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="2">
+        <v>458</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="H73" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H73" s="2" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" s="2" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B74" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Erträge aus anderen Wertpapieren (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I74)," (",G74," - ",H74,")")</f>
+        <v>Sonstige Zinsen und ähnliche Erträge (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="2">
+        <v>459</v>
+      </c>
+      <c r="G74" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" s="2" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B75" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige Zinsen und ähnliche Erträge (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I75)," (",G75," - ",H75,")")</f>
+        <v>Abschreibungen auf Finanzanlagen (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="2">
+        <v>460</v>
+      </c>
+      <c r="G75" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="H75" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H75" s="2" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" s="2" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B76" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Abschreibungen auf Finanzanlagen (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I76)," (",G76," - ",H76,")")</f>
+        <v>Zinsen und ähnliche Aufwendungen (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="2">
+        <v>461</v>
+      </c>
+      <c r="G76" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B77" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Zinsen und ähnliche Aufwendungen (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I77)," (",G77," - ",H77,")")</f>
+        <v>Sonstige Steuern (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="F77" s="2">
+        <v>462</v>
+      </c>
+      <c r="G77" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="H77" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>882</v>
+        <v>792</v>
       </c>
       <c r="B78" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonstige Steuern (Geschäftsbetrieb - Ausgaben)</v>
+        <f>_xlfn.CONCAT(TRIM(I78)," (",G78," - ",H78,")")</f>
+        <v>Gesamt (Geschäftsbetrieb - Ausgaben)</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="E78" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D78" s="2" t="str" cm="1">
+        <f t="array" ref="D78">_xlfn.TEXTJOIN(" + ", TRUE, _xlfn._xlws.FILTER(A:A, (LEFT(A:A, LEN(A78))=A78) * (A:A&lt;&gt;A78)))</f>
+        <v>GBAUS1 + GBAUS2 + GBAUS3 + GBAUS4 + GBAUS5 + GBAUS6 + GBAUS7 + GBAUS8 + GBAUS9 + GBAUS10 + GBAUS11 + GBAUS12 + GBAUS13</v>
+      </c>
+      <c r="F78" s="2">
+        <v>499</v>
+      </c>
+      <c r="G78" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="H78" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>786</v>
+      <c r="I78" s="2" t="s">
+        <v>754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>